<commit_message>
updated smoking cessation codelists
</commit_message>
<xml_diff>
--- a/codelists/Smoking_cessation_behavioural_SNOMED.xlsx
+++ b/codelists/Smoking_cessation_behavioural_SNOMED.xlsx
@@ -1,33 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" firstSheet="0" windowHeight="13125" windowWidth="13125" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -52,17 +42,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -77,44 +63,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -141,14 +127,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -175,6 +179,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -186,179 +208,175 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
+            <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="1" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8.43" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>conceptId</t>
         </is>
@@ -367,7 +385,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>185789006</t>
+          <t>711028002</t>
         </is>
       </c>
     </row>
@@ -381,144 +399,132 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>315232003</t>
+          <t>225324006</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>384742004</t>
+          <t>401068004</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>390900001</t>
+          <t>401160008</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>390901002</t>
+          <t>506491000000102</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>395700008</t>
+          <t>712971000000108</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>401068004</t>
+          <t>384742004</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>401160008</t>
+          <t>200221000000105</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>200221000000105</t>
+          <t>201931000000109</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>374361000000100</t>
+          <t>201941000000100</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>374391000000106</t>
+          <t>1110791000000100</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>505281000000106</t>
+          <t>1659131000000104</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>505581000000108</t>
+          <t>521721000000109</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>506491000000102</t>
+          <t>699033005</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>712971000000108</t>
+          <t>702388001</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>714001000000108</t>
+          <t>712829007</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>750821000000109</t>
+          <t>771155005</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>750851000000104</t>
+          <t>838131000000103</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>755721000000107</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>783011000000105</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>871661000000106</t>
+          <t>171055003</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>